<commit_message>
fix issue so dryness is reattributed every run
</commit_message>
<xml_diff>
--- a/Wildfire_Burning_Alg.xlsx
+++ b/Wildfire_Burning_Alg.xlsx
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -511,10 +511,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -568,10 +568,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -587,10 +587,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -606,10 +606,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -625,10 +625,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -644,10 +644,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -663,10 +663,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -682,10 +682,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -701,10 +701,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -720,10 +720,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -739,10 +739,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -758,10 +758,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -777,10 +777,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
@@ -796,10 +796,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -815,10 +815,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -834,10 +834,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -853,10 +853,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
@@ -872,10 +872,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -891,10 +891,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -910,10 +910,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -929,10 +929,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
@@ -948,10 +948,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -967,10 +967,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
@@ -986,10 +986,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -1024,10 +1024,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -1043,10 +1043,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
@@ -1062,10 +1062,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
@@ -1081,10 +1081,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
@@ -1100,10 +1100,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
@@ -1119,10 +1119,10 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37">
@@ -1138,10 +1138,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1157,10 +1157,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1176,10 +1176,10 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1195,10 +1195,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41">
@@ -1214,10 +1214,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42">
@@ -1233,10 +1233,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -1252,10 +1252,10 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
@@ -1271,10 +1271,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
@@ -1290,10 +1290,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
@@ -1309,10 +1309,10 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E46" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47">
@@ -1328,10 +1328,10 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
@@ -1347,10 +1347,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E48" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49">
@@ -1366,10 +1366,10 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -1385,10 +1385,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
@@ -1404,10 +1404,10 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.271264367816092</v>
+        <v>0.3379310344827586</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added clustering, and eccentricity from starting node + cleaned up code
</commit_message>
<xml_diff>
--- a/Wildfire_Burning_Alg.xlsx
+++ b/Wildfire_Burning_Alg.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>nx,average_clustering(G)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>nx.eccentricity(G,starting_node)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>steps</t>
         </is>
       </c>
@@ -473,10 +483,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -492,10 +508,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -511,10 +533,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -530,10 +558,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -549,9 +583,15 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E6" t="n">
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="n">
         <v>9</v>
       </c>
     </row>
@@ -568,10 +608,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -587,10 +633,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -606,10 +658,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -625,10 +683,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -644,10 +708,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -663,9 +733,15 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E12" t="n">
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="n">
         <v>7</v>
       </c>
     </row>
@@ -682,9 +758,15 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E13" t="n">
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
         <v>8</v>
       </c>
     </row>
@@ -701,10 +783,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -720,10 +808,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -739,9 +833,15 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E16" t="n">
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" t="n">
         <v>8</v>
       </c>
     </row>
@@ -758,10 +858,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E17" t="n">
-        <v>12</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -777,10 +883,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E18" t="n">
-        <v>11</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="19">
@@ -796,10 +908,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
@@ -815,10 +933,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E20" t="n">
-        <v>6</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="21">
@@ -834,10 +958,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="22">
@@ -853,10 +983,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E22" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -872,10 +1008,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -891,10 +1033,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="25">
@@ -910,10 +1058,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="26">
@@ -929,10 +1083,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G26" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="27">
@@ -948,10 +1108,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E27" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3</v>
+      </c>
+      <c r="G27" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="28">
@@ -967,9 +1133,15 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E28" t="n">
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3</v>
+      </c>
+      <c r="G28" t="n">
         <v>13</v>
       </c>
     </row>
@@ -986,10 +1158,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E29" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G29" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="30">
@@ -1005,10 +1183,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="31">
@@ -1024,10 +1208,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="32">
@@ -1043,9 +1233,15 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E32" t="n">
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G32" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1062,10 +1258,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E33" t="n">
-        <v>13</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="34">
@@ -1081,10 +1283,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="35">
@@ -1100,10 +1308,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3</v>
+      </c>
+      <c r="G35" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="36">
@@ -1119,10 +1333,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E36" t="n">
-        <v>9</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="37">
@@ -1138,9 +1358,15 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E37" t="n">
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1157,10 +1383,16 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3</v>
+      </c>
+      <c r="G38" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="39">
@@ -1176,10 +1408,16 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E39" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2</v>
+      </c>
+      <c r="G39" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -1195,10 +1433,16 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E40" t="n">
-        <v>9</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2</v>
+      </c>
+      <c r="G40" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="41">
@@ -1214,10 +1458,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E41" t="n">
-        <v>10</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3</v>
+      </c>
+      <c r="G41" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="42">
@@ -1233,10 +1483,16 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E42" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="43">
@@ -1252,10 +1508,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3</v>
+      </c>
+      <c r="G43" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="44">
@@ -1271,10 +1533,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E44" t="n">
-        <v>8</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2</v>
+      </c>
+      <c r="G44" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="45">
@@ -1290,10 +1558,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E45" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="46">
@@ -1309,10 +1583,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E46" t="n">
-        <v>12</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2</v>
+      </c>
+      <c r="G46" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="47">
@@ -1328,10 +1608,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E47" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3</v>
+      </c>
+      <c r="G47" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="48">
@@ -1347,10 +1633,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E48" t="n">
-        <v>6</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="49">
@@ -1366,10 +1658,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E49" t="n">
-        <v>14</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="50">
@@ -1385,10 +1683,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E50" t="n">
-        <v>7</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F50" t="n">
+        <v>3</v>
+      </c>
+      <c r="G50" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="51">
@@ -1404,10 +1708,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.3379310344827586</v>
+        <v>0.3057471264367816</v>
       </c>
       <c r="E51" t="n">
-        <v>9</v>
+        <v>0.3085360935360936</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3</v>
+      </c>
+      <c r="G51" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>